<commit_message>
regular Schedule Data Sheet
</commit_message>
<xml_diff>
--- a/src/test/java/com/pack/testData/RegularShedules.xlsx
+++ b/src/test/java/com/pack/testData/RegularShedules.xlsx
@@ -61,7 +61,7 @@
     <t>DoubleClickDay</t>
   </si>
   <si>
-    <t xml:space="preserve">StartTime1
+    <t xml:space="preserve">StartTime1
 </t>
   </si>
   <si>
@@ -110,18 +110,18 @@
     <t>Week Day1</t>
   </si>
   <si>
-    <t xml:space="preserve">StartTime
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week Day1
+    <t xml:space="preserve">StartTime
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week Day1
 </t>
   </si>
   <si>
     <t>Week Day2</t>
   </si>
   <si>
-    <t xml:space="preserve">Week Day3
+    <t xml:space="preserve">Week Day3
 </t>
   </si>
   <si>
@@ -165,13 +165,174 @@
   </si>
   <si>
     <t>Variable</t>
+  </si>
+  <si>
+    <t>6:00AM</t>
+  </si>
+  <si>
+    <t>2:00PM</t>
+  </si>
+  <si>
+    <t>TUESADY</t>
+  </si>
+  <si>
+    <t>5:00AM</t>
+  </si>
+  <si>
+    <t>2:PM</t>
+  </si>
+  <si>
+    <t>SATURDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEDNESDAY
+</t>
+  </si>
+  <si>
+    <t>8:00PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SATURDAY
+</t>
+  </si>
+  <si>
+    <t>10:PM</t>
+  </si>
+  <si>
+    <t>tTHUSDAY</t>
+  </si>
+  <si>
+    <t>THUSDAY</t>
+  </si>
+  <si>
+    <t>Salaried</t>
+  </si>
+  <si>
+    <t>7:00AM</t>
+  </si>
+  <si>
+    <t>3:PM</t>
+  </si>
+  <si>
+    <t>3:00PM</t>
+  </si>
+  <si>
+    <t>STURDAY</t>
+  </si>
+  <si>
+    <t>10:00PM</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>10:00AM</t>
+  </si>
+  <si>
+    <t>9:00PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salaried
+</t>
+  </si>
+  <si>
+    <t>11:00AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supervisor
+</t>
+  </si>
+  <si>
+    <t>12:00AM</t>
+  </si>
+  <si>
+    <t>11:00PM</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable
+</t>
+  </si>
+  <si>
+    <t>1:00AM</t>
+  </si>
+  <si>
+    <t>TUES</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEDNESDAY
+</t>
+  </si>
+  <si>
+    <t>12:00PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRIDAY
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONDAY
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUNDAY
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONDAY
+</t>
+  </si>
+  <si>
+    <t>Week day4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SATURDAY
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRIDAY
+</t>
+  </si>
+  <si>
+    <t>TESDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEDNESDAY
+</t>
+  </si>
+  <si>
+    <t>wEDNESDAY</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>DoubleClickDay(dAY3)</t>
+  </si>
+  <si>
+    <t>StartTime1</t>
+  </si>
+  <si>
+    <t>Week Day3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,16 +340,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -196,12 +372,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment wrapText="1" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,184 +722,675 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection activeCell="A3" sqref="A3" activeCellId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="L1">
+      <selection activeCell="L4" sqref="L4:Z4" activeCellId="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.4531" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" width="11.4531" customWidth="1" bestFit="1"/>
     <col min="6" max="6" width="13.6328" customWidth="1" bestFit="1"/>
     <col min="7" max="7" width="10.9062" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" width="12" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" width="12.543" customWidth="1" bestFit="1"/>
     <col min="10" max="10" width="12.543" customWidth="1" bestFit="1"/>
     <col min="11" max="11" width="11.7266" customWidth="1" bestFit="1"/>
     <col min="12" max="12" width="10" customWidth="1" bestFit="1"/>
     <col min="13" max="13" width="9.17969" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" width="10.2695" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" width="10.2695" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" width="11.1797" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" width="10" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" width="10.9062" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" width="10.9062" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" width="10" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" width="9.17969" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" width="13.3633" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" width="11.4531" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" width="11.4531" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" width="12.543" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" width="12.543" customWidth="1"/>
+    <col min="18" max="18" width="11.4531" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" width="10" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" width="11.4531" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" width="12.543" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" width="10" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" width="9.17969" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" width="11.4531" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" width="13.3633" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" s="0" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>987816</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="0">
+        <v>5437</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="P2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>987817</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="F3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
-        <v>18</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="J3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="T2" t="s">
+      <c r="M3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>999887</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="U2" t="s">
-        <v>9</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="R4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>585278</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>585211</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>635677</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="W2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="N7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="Y2" t="s">
-        <v>44</v>
+      <c r="P7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>787887</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="V8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="W8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>